<commit_message>
Implements head activation section
</commit_message>
<xml_diff>
--- a/data/ESLO/all_selected_data/ESLO1_quoi_questions.xlsx
+++ b/data/ESLO/all_selected_data/ESLO1_quoi_questions.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinabonan/Desktop/GitHubRepos/parameters-corpus-work/data/ESLO/all_selected_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCE1D76-0658-4245-9C74-D82A5CEFD6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B85B00E-B7CC-B141-931B-C31C5CF091A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-65880" yWindow="-10300" windowWidth="51160" windowHeight="28160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="172" r:id="rId2"/>
+    <pivotCache cacheId="33" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -4307,6 +4307,27 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="90000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:srgbClr val="4F81BD">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="40000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
             <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -4334,23 +4355,17 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$AG$7:$AH$11</c:f>
+              <c:f>(Sheet1!$AG$8:$AH$8,Sheet1!$AG$10:$AH$11)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>que</c:v>
+                    <c:v>VS</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>VS</c:v>
+                    <c:v>SV</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>est-ce que</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>SV</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
                     <c:v>SV</c:v>
                   </c:pt>
                 </c:lvl>
@@ -4362,12 +4377,6 @@
                     <c:v>ex situ</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>ex situ</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>ex situ</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
                     <c:v>in situ</c:v>
                   </c:pt>
                 </c:lvl>
@@ -4376,23 +4385,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AI$7:$AI$11</c:f>
+              <c:f>(Sheet1!$AI$8,Sheet1!$AI$10:$AI$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>217</c:v>
                 </c:pt>
               </c:numCache>
@@ -9187,7 +9190,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{626D8E16-C070-E446-A88D-32466A837D7F}" name="PivotTable12" cacheId="172" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{626D8E16-C070-E446-A88D-32466A837D7F}" name="PivotTable12" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="N4:O22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -9592,7 +9595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI694"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="144" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="144" workbookViewId="0">
       <selection activeCell="AK6" sqref="AK6"/>
     </sheetView>
   </sheetViews>

</xml_diff>